<commit_message>
Refactored services, validators and controllers
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Аксенчиков Леонид Викторович</t>
   </si>
@@ -27,40 +30,88 @@
     <t>водитель</t>
   </si>
   <si>
-    <t>Асмоловский Евгений Валерьевич</t>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Ашомко Виталий Романович</t>
+  </si>
+  <si>
+    <t>Базылев Леонид Иванович</t>
+  </si>
+  <si>
+    <t>Балюко Вячеслав Иванович</t>
+  </si>
+  <si>
+    <t>Барталевич Григорий Александрович</t>
+  </si>
+  <si>
+    <t>Белоус Алексей Олегович</t>
+  </si>
+  <si>
+    <t>Бондаренко Павел Павлович</t>
+  </si>
+  <si>
+    <t>Бугримов Олег Александрович</t>
+  </si>
+  <si>
+    <t>водитель погрузчика</t>
+  </si>
+  <si>
+    <t>Вальков Андрей Петрович</t>
   </si>
   <si>
     <t>тракторист</t>
   </si>
   <si>
-    <t>Ашомко Виталий Романович</t>
-  </si>
-  <si>
-    <t>Базылев Леонид Иванович</t>
-  </si>
-  <si>
-    <t>Балюко Вячеслав Иванович</t>
-  </si>
-  <si>
-    <t>Барталевич Григорий Александрович</t>
-  </si>
-  <si>
-    <t>Белоус Алексей Олегович</t>
-  </si>
-  <si>
-    <t>Бондаренко Павел Павлович</t>
-  </si>
-  <si>
-    <t>Бугримов Олег Александрович</t>
-  </si>
-  <si>
-    <t>водитель погрузчика</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Position</t>
+    <t>Гавриленко Виктор Александрович</t>
+  </si>
+  <si>
+    <t>Гаврилин Игорь Владимирович</t>
+  </si>
+  <si>
+    <t>Герасимов Денис Сергеевич</t>
+  </si>
+  <si>
+    <t>Героимов Геннадий Борисович</t>
+  </si>
+  <si>
+    <t>Глазов Дмитрий Алексеевич</t>
+  </si>
+  <si>
+    <t>Голубев Константин Александрович</t>
+  </si>
+  <si>
+    <t>Голубков Игорь Николаевич</t>
+  </si>
+  <si>
+    <t>Гольяшов Виталий Александрович</t>
+  </si>
+  <si>
+    <t>Горохов Юрий Владимирович</t>
+  </si>
+  <si>
+    <t>Григорьев Сергей Геннадьевич</t>
+  </si>
+  <si>
+    <t>машинист трактора</t>
+  </si>
+  <si>
+    <t>Громыко Андрей Викторович</t>
+  </si>
+  <si>
+    <t>Гусаков Георгий Михайлович</t>
+  </si>
+  <si>
+    <t>Даронько Александр Михайлович</t>
+  </si>
+  <si>
+    <t>Дашук Игорь Владимирович</t>
+  </si>
+  <si>
+    <t>Двороковский Кирилл Анатольевич</t>
   </si>
 </sst>
 </file>
@@ -103,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -111,11 +162,84 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -199,8 +323,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -250,7 +374,75 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="689610" y="1091565"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Сверка"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,10 +721,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,15 +737,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -561,23 +753,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -585,7 +777,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
@@ -593,25 +785,145 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A2:B10" name="Диапазон1"/>
+    <protectedRange sqref="A2:B25" name="Диапазон1_1"/>
   </protectedRanges>
-  <conditionalFormatting sqref="A2:B10">
+  <conditionalFormatting sqref="A2:B25">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>OR(AND($G2&lt;&gt;"",$G2&lt;TODAY()),AND($E2&lt;&gt;"",$E2&lt;TODAY()))</formula>
     </cfRule>
@@ -629,9 +941,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Z:\Данные по ГорСАП\.db\ГАИ\[Учет действия водительских удостоверений и медицинских справок(проверен).xlsm]Сверка'!#REF!</xm:f>
+            <xm:f>'[Учет действия водительских удостоверений и медицинских справок.xlsm]Сверка'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B10</xm:sqref>
+          <xm:sqref>B2:B25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>